<commit_message>
add feature find by field for customer
</commit_message>
<xml_diff>
--- a/MilkTeaSalesSystem.xlsx
+++ b/MilkTeaSalesSystem.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01_Java\09_Hibernate\04_SourceCode\MilkTeaSalesSystem\MilkTeaSalesSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B5F1B8-3368-47BF-9C75-41F5E30463FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1497FAE-DD4A-4D54-B866-40FCE368AD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="2" r:id="rId1"/>
-    <sheet name="Store" sheetId="1" r:id="rId2"/>
-    <sheet name="Order" sheetId="3" r:id="rId3"/>
-    <sheet name="MilkTea" sheetId="4" r:id="rId4"/>
-    <sheet name="Topping" sheetId="5" r:id="rId5"/>
-    <sheet name="OrderTopping" sheetId="6" r:id="rId6"/>
-    <sheet name="OrderMilkTea" sheetId="7" r:id="rId7"/>
+    <sheet name="Find_Customer" sheetId="8" r:id="rId2"/>
+    <sheet name="Store" sheetId="1" r:id="rId3"/>
+    <sheet name="Order" sheetId="3" r:id="rId4"/>
+    <sheet name="MilkTea" sheetId="4" r:id="rId5"/>
+    <sheet name="Topping" sheetId="5" r:id="rId6"/>
+    <sheet name="OrderTopping" sheetId="6" r:id="rId7"/>
+    <sheet name="OrderMilkTea" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
   <si>
     <t>StoreId</t>
   </si>
@@ -117,24 +118,6 @@
     <t>f@gmail.com</t>
   </si>
   <si>
-    <t>328150801</t>
-  </si>
-  <si>
-    <t>328150802</t>
-  </si>
-  <si>
-    <t>328150803</t>
-  </si>
-  <si>
-    <t>328150804</t>
-  </si>
-  <si>
-    <t>328150805</t>
-  </si>
-  <si>
-    <t>328150806</t>
-  </si>
-  <si>
     <t>OrderId</t>
   </si>
   <si>
@@ -250,6 +233,33 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>What do you want to find?</t>
+  </si>
+  <si>
+    <t>Your input</t>
+  </si>
+  <si>
+    <t>0328150801</t>
+  </si>
+  <si>
+    <t>0328150802</t>
+  </si>
+  <si>
+    <t>0328150803</t>
+  </si>
+  <si>
+    <t>0328150804</t>
+  </si>
+  <si>
+    <t>0328150805</t>
+  </si>
+  <si>
+    <t>0328150806</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -588,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +641,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -648,7 +658,7 @@
         <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,7 +675,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -682,7 +692,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -699,7 +709,7 @@
         <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,7 +726,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -734,6 +744,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8DBC4B-C190-4478-90BC-CD8460359F2F}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{5F50B6CE-38CC-44AA-8C2A-298889632A00}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -773,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -787,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -801,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -810,7 +883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -829,16 +902,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -852,10 +925,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="D2">
         <v>100000</v>
@@ -872,10 +945,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D3">
         <v>200000</v>
@@ -892,10 +965,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>300000</v>
@@ -912,10 +985,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>400000</v>
@@ -932,10 +1005,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D6">
         <v>500000</v>
@@ -952,10 +1025,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D7">
         <v>600000</v>
@@ -973,7 +1046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -989,13 +1062,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>10000</v>
@@ -1014,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>20000</v>
@@ -1025,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>50000</v>
@@ -1036,7 +1109,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>10000</v>
@@ -1047,7 +1120,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>50000</v>
@@ -1058,7 +1131,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>20000</v>
@@ -1069,7 +1142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1085,13 +1158,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>5000</v>
@@ -1110,7 +1183,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>10000</v>
@@ -1121,7 +1194,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>20000</v>
@@ -1132,7 +1205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1148,100 +1221,100 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1265,100 +1338,100 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add feature find by field
</commit_message>
<xml_diff>
--- a/MilkTeaSalesSystem.xlsx
+++ b/MilkTeaSalesSystem.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01_Java\09_Hibernate\04_SourceCode\MilkTeaSalesSystem\MilkTeaSalesSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1497FAE-DD4A-4D54-B866-40FCE368AD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A486D7-A04A-47AF-853D-C487556E3C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="2" r:id="rId1"/>
     <sheet name="Find_Customer" sheetId="8" r:id="rId2"/>
     <sheet name="Store" sheetId="1" r:id="rId3"/>
-    <sheet name="Order" sheetId="3" r:id="rId4"/>
-    <sheet name="MilkTea" sheetId="4" r:id="rId5"/>
-    <sheet name="Topping" sheetId="5" r:id="rId6"/>
-    <sheet name="OrderTopping" sheetId="6" r:id="rId7"/>
-    <sheet name="OrderMilkTea" sheetId="7" r:id="rId8"/>
+    <sheet name="Find_Store" sheetId="9" r:id="rId4"/>
+    <sheet name="Order" sheetId="3" r:id="rId5"/>
+    <sheet name="Find_Order" sheetId="11" r:id="rId6"/>
+    <sheet name="MilkTea" sheetId="4" r:id="rId7"/>
+    <sheet name="Find_MilkTea" sheetId="10" r:id="rId8"/>
+    <sheet name="Topping" sheetId="5" r:id="rId9"/>
+    <sheet name="Find_Topping" sheetId="12" r:id="rId10"/>
+    <sheet name="OrderTopping" sheetId="6" r:id="rId11"/>
+    <sheet name="OrderMilkTea" sheetId="7" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="80">
   <si>
     <t>StoreId</t>
   </si>
@@ -235,9 +239,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>What do you want to find?</t>
-  </si>
-  <si>
     <t>Your input</t>
   </si>
   <si>
@@ -260,6 +261,21 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>What do you looking for?</t>
+  </si>
+  <si>
+    <t>Price[greater than or equal]</t>
+  </si>
+  <si>
+    <t>Price[less than or equal]</t>
+  </si>
+  <si>
+    <t>TotalPrice[greater than or equal]</t>
+  </si>
+  <si>
+    <t>TotalPrice[less than or equal]</t>
   </si>
 </sst>
 </file>
@@ -641,7 +657,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -658,7 +674,7 @@
         <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -675,7 +691,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -692,7 +708,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -709,7 +725,7 @@
         <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,7 +742,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -743,12 +759,298 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A364D3B3-2931-48E8-A4E8-B14947E35CBA}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8DBC4B-C190-4478-90BC-CD8460359F2F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,10 +1062,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -771,7 +1073,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -787,7 +1089,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -811,7 +1113,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,11 +1186,62 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAA6CB1-62EF-4903-B853-FB38C200C2F9}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,12 +1399,87 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DF1ACF-D2E2-484C-9B50-013EE9B1D879}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1570,58 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9286217-E656-4A24-B518-3755E8BA6157}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="2">
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1203,239 +1682,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
finish feature update for all entity
</commit_message>
<xml_diff>
--- a/MilkTeaSalesSystem.xlsx
+++ b/MilkTeaSalesSystem.xlsx
@@ -8,23 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01_Java\09_Hibernate\04_SourceCode\MilkTeaSalesSystem\MilkTeaSalesSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A486D7-A04A-47AF-853D-C487556E3C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE18AE85-606D-487D-9D9A-F18CC68FBFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="916" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="2" r:id="rId1"/>
     <sheet name="Find_Customer" sheetId="8" r:id="rId2"/>
-    <sheet name="Store" sheetId="1" r:id="rId3"/>
-    <sheet name="Find_Store" sheetId="9" r:id="rId4"/>
-    <sheet name="Order" sheetId="3" r:id="rId5"/>
-    <sheet name="Find_Order" sheetId="11" r:id="rId6"/>
-    <sheet name="MilkTea" sheetId="4" r:id="rId7"/>
-    <sheet name="Find_MilkTea" sheetId="10" r:id="rId8"/>
-    <sheet name="Topping" sheetId="5" r:id="rId9"/>
-    <sheet name="Find_Topping" sheetId="12" r:id="rId10"/>
-    <sheet name="OrderTopping" sheetId="6" r:id="rId11"/>
-    <sheet name="OrderMilkTea" sheetId="7" r:id="rId12"/>
+    <sheet name="Update_Customer" sheetId="13" r:id="rId3"/>
+    <sheet name="Store" sheetId="1" r:id="rId4"/>
+    <sheet name="Find_Store" sheetId="9" r:id="rId5"/>
+    <sheet name="Update_Store" sheetId="14" r:id="rId6"/>
+    <sheet name="Order" sheetId="3" r:id="rId7"/>
+    <sheet name="Find_Order" sheetId="11" r:id="rId8"/>
+    <sheet name="Update_Order" sheetId="15" r:id="rId9"/>
+    <sheet name="MilkTea" sheetId="4" r:id="rId10"/>
+    <sheet name="Find_MilkTea" sheetId="10" r:id="rId11"/>
+    <sheet name="Update_MilkTea" sheetId="16" r:id="rId12"/>
+    <sheet name="Topping" sheetId="5" r:id="rId13"/>
+    <sheet name="Find_Topping" sheetId="12" r:id="rId14"/>
+    <sheet name="Update_Topping" sheetId="17" r:id="rId15"/>
+    <sheet name="OrderTopping" sheetId="6" r:id="rId16"/>
+    <sheet name="OrderMilkTea" sheetId="7" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="96">
   <si>
     <t>StoreId</t>
   </si>
@@ -276,6 +281,54 @@
   </si>
   <si>
     <t>TotalPrice[less than or equal]</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>Store AAA</t>
+  </si>
+  <si>
+    <t>Store BBB</t>
+  </si>
+  <si>
+    <t>Milk tea aaa</t>
+  </si>
+  <si>
+    <t>Milk tea bbb</t>
+  </si>
+  <si>
+    <t>Milk tea ccc</t>
+  </si>
+  <si>
+    <t>Topping aaa</t>
+  </si>
+  <si>
+    <t>Topping bbb</t>
+  </si>
+  <si>
+    <t>29/09/2222</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>100000</t>
   </si>
 </sst>
 </file>
@@ -326,11 +379,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -615,7 +669,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A2" sqref="A2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,11 +814,285 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9286217-E656-4A24-B518-3755E8BA6157}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D050DA2-CF9D-4FE6-AF0B-4EFB4F21CB42}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A364D3B3-2931-48E8-A4E8-B14947E35CBA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,16 +1121,16 @@
       <c r="A3" t="s">
         <v>76</v>
       </c>
-      <c r="B3">
-        <v>5000</v>
+      <c r="B3" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
-      <c r="B4">
-        <v>5000</v>
+      <c r="B4" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -810,7 +1138,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B938508C-78D3-4F35-BF99-5030067A9646}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -928,7 +1309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1050,7 +1431,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,11 +1490,106 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA052CA-3764-4BAF-962D-D281ACCF562C}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{66AAA4EE-CD3B-4907-90E2-3C9245D51DD2}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{8EDA6902-0587-4527-BD4E-8FC0BD9B8496}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{F95E7456-4267-4A60-8CEE-F44380951175}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAA6CB1-62EF-4903-B853-FB38C200C2F9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1236,12 +1712,75 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C60CB6-B39B-4FA8-A1F4-6234DFECC786}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1816,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1297,7 +1836,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1317,7 +1856,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1337,7 +1876,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1357,7 +1896,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1377,7 +1916,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1399,12 +1938,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DF1ACF-D2E2-484C-9B50-013EE9B1D879}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,209 +2013,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C7"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18F2EAE-8E7F-424D-B553-4B8E5E6930AD}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>100000</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3">
+        <v>200000</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7">
-        <v>20000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9286217-E656-4A24-B518-3755E8BA6157}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="2">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="2">
-        <v>100000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="B4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4">
+        <v>300000</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F4">
         <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4">
-        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>